<commit_message>
Added a second house column, to reflect someone moving from one House to another via marriage. Also, a 'kingdom' column
</commit_message>
<xml_diff>
--- a/got_popular_chars-Baelor-1.xlsx
+++ b/got_popular_chars-Baelor-1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="615" yWindow="3615" windowWidth="27990" windowHeight="8655"/>
+    <workbookView xWindow="-1305" yWindow="1770" windowWidth="27990" windowHeight="8655"/>
   </bookViews>
   <sheets>
     <sheet name="characters" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="248">
   <si>
     <t>name</t>
   </si>
@@ -129,9 +129,6 @@
     <t>Robb Stark</t>
   </si>
   <si>
-    <t>Catelyn Stark</t>
-  </si>
-  <si>
     <t>Eddard Stark</t>
   </si>
   <si>
@@ -381,9 +378,6 @@
     <t>Dorna Swyft</t>
   </si>
   <si>
-    <t>Lysa Arryn</t>
-  </si>
-  <si>
     <t>Mance Rayder</t>
   </si>
   <si>
@@ -714,7 +708,58 @@
     <t>killer</t>
   </si>
   <si>
-    <t>Olenna Tyrell</t>
+    <t>kingdom</t>
+  </si>
+  <si>
+    <t>second house</t>
+  </si>
+  <si>
+    <t>Riverlands</t>
+  </si>
+  <si>
+    <t>Hoster Tully</t>
+  </si>
+  <si>
+    <t>Walder Rivers</t>
+  </si>
+  <si>
+    <t>(House Targaryen)</t>
+  </si>
+  <si>
+    <t>Lysa Tully</t>
+  </si>
+  <si>
+    <t>Olenna Redwyne</t>
+  </si>
+  <si>
+    <t>Crownlands</t>
+  </si>
+  <si>
+    <t>Reach</t>
+  </si>
+  <si>
+    <t>North</t>
+  </si>
+  <si>
+    <t>Stormlands</t>
+  </si>
+  <si>
+    <t>Westerlands</t>
+  </si>
+  <si>
+    <t>Iron Islands</t>
+  </si>
+  <si>
+    <t>Vale</t>
+  </si>
+  <si>
+    <t>Essos</t>
+  </si>
+  <si>
+    <t>Dorne</t>
+  </si>
+  <si>
+    <t>Beyond the Wall</t>
   </si>
 </sst>
 </file>
@@ -1047,9 +1092,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q69"/>
+  <dimension ref="A1:S70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M27" sqref="M27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -1061,20 +1108,22 @@
     <col min="6" max="6" width="48.28515625" customWidth="1"/>
     <col min="7" max="7" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="30.5703125" customWidth="1"/>
-    <col min="14" max="14" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="39" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="38.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="23" customWidth="1"/>
+    <col min="9" max="9" width="23.42578125" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="30.5703125" customWidth="1"/>
+    <col min="15" max="15" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="39" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="39" customWidth="1"/>
+    <col min="18" max="18" width="38.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:19">
       <c r="A1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B1" t="s">
         <v>11</v>
@@ -1086,46 +1135,52 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="H1" t="s">
         <v>2</v>
       </c>
       <c r="I1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J1" t="s">
         <v>3</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>4</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>5</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>6</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>7</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>8</v>
-      </c>
-      <c r="P1" t="s">
-        <v>9</v>
       </c>
       <c r="Q1" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="2" spans="1:17">
+      <c r="R1" t="s">
+        <v>9</v>
+      </c>
+      <c r="S1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
       <c r="A2">
         <v>6</v>
       </c>
@@ -1136,34 +1191,37 @@
         <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>208</v>
-      </c>
-      <c r="L2" t="s">
+        <v>206</v>
+      </c>
+      <c r="I2" t="s">
+        <v>238</v>
+      </c>
+      <c r="M2" t="s">
         <v>20</v>
       </c>
-      <c r="M2" t="s">
-        <v>160</v>
-      </c>
       <c r="N2" t="s">
+        <v>158</v>
+      </c>
+      <c r="O2" t="s">
         <v>22</v>
       </c>
-      <c r="O2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17">
+      <c r="P2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
       <c r="A3">
         <v>51</v>
       </c>
@@ -1174,34 +1232,37 @@
         <v>30</v>
       </c>
       <c r="D3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="F3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>208</v>
-      </c>
-      <c r="L3" t="s">
+        <v>206</v>
+      </c>
+      <c r="I3" t="s">
+        <v>238</v>
+      </c>
+      <c r="M3" t="s">
         <v>20</v>
       </c>
-      <c r="M3" t="s">
-        <v>160</v>
-      </c>
       <c r="N3" t="s">
+        <v>158</v>
+      </c>
+      <c r="O3" t="s">
         <v>19</v>
       </c>
-      <c r="O3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17">
+      <c r="P3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
       <c r="A4">
         <v>55</v>
       </c>
@@ -1212,34 +1273,34 @@
         <v>31</v>
       </c>
       <c r="E4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G4">
         <v>0</v>
       </c>
       <c r="H4" t="s">
-        <v>208</v>
-      </c>
-      <c r="I4">
+        <v>206</v>
+      </c>
+      <c r="I4" t="s">
+        <v>239</v>
+      </c>
+      <c r="J4">
         <v>283</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>22</v>
       </c>
-      <c r="M4" t="s">
-        <v>90</v>
-      </c>
-      <c r="O4" t="s">
+      <c r="N4" t="s">
+        <v>89</v>
+      </c>
+      <c r="P4" t="s">
         <v>32</v>
       </c>
-      <c r="P4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17">
+    </row>
+    <row r="5" spans="1:19">
       <c r="A5">
         <v>102</v>
       </c>
@@ -1250,31 +1311,34 @@
         <v>36</v>
       </c>
       <c r="D5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E5" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="F5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G5">
         <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>163</v>
-      </c>
-      <c r="L5" t="s">
+        <v>161</v>
+      </c>
+      <c r="I5" t="s">
+        <v>240</v>
+      </c>
+      <c r="M5" t="s">
+        <v>106</v>
+      </c>
+      <c r="N5" t="s">
         <v>37</v>
       </c>
-      <c r="M5" t="s">
-        <v>38</v>
-      </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:19">
       <c r="A6">
         <v>173</v>
       </c>
@@ -1282,40 +1346,43 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" t="s">
+        <v>211</v>
+      </c>
+      <c r="E6" t="s">
+        <v>210</v>
+      </c>
+      <c r="F6" t="s">
+        <v>142</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6" t="s">
+        <v>206</v>
+      </c>
+      <c r="I6" t="s">
+        <v>241</v>
+      </c>
+      <c r="M6" t="s">
         <v>47</v>
       </c>
-      <c r="D6" t="s">
-        <v>213</v>
-      </c>
-      <c r="E6" t="s">
-        <v>212</v>
-      </c>
-      <c r="F6" t="s">
-        <v>144</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-      <c r="H6" t="s">
-        <v>208</v>
-      </c>
-      <c r="L6" t="s">
+      <c r="N6" t="s">
         <v>48</v>
       </c>
-      <c r="M6" t="s">
+      <c r="O6" t="s">
         <v>49</v>
       </c>
-      <c r="N6" t="s">
-        <v>50</v>
-      </c>
-      <c r="O6" t="s">
-        <v>59</v>
-      </c>
       <c r="P6" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17">
+        <v>58</v>
+      </c>
+      <c r="R6" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19">
       <c r="A7">
         <v>1467</v>
       </c>
@@ -1323,37 +1390,40 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E7" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="F7" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
       <c r="H7" t="s">
-        <v>163</v>
-      </c>
-      <c r="I7">
+        <v>161</v>
+      </c>
+      <c r="I7" t="s">
+        <v>240</v>
+      </c>
+      <c r="J7">
         <v>289</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>16</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
+        <v>106</v>
+      </c>
+      <c r="N7" t="s">
         <v>37</v>
       </c>
-      <c r="M7" t="s">
-        <v>38</v>
-      </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:19">
       <c r="A8">
         <v>1475</v>
       </c>
@@ -1361,37 +1431,40 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F8" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G8">
         <v>1</v>
       </c>
       <c r="H8" t="s">
-        <v>163</v>
-      </c>
-      <c r="I8">
+        <v>161</v>
+      </c>
+      <c r="I8" t="s">
+        <v>240</v>
+      </c>
+      <c r="J8">
         <v>290</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>15</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
+        <v>106</v>
+      </c>
+      <c r="N8" t="s">
         <v>37</v>
       </c>
-      <c r="M8" t="s">
-        <v>38</v>
-      </c>
-      <c r="O8" t="s">
+      <c r="P8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:19">
       <c r="A9">
         <v>1482</v>
       </c>
@@ -1405,37 +1478,43 @@
         <v>17</v>
       </c>
       <c r="E9" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F9" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G9">
         <v>0</v>
       </c>
       <c r="H9" t="s">
-        <v>208</v>
-      </c>
-      <c r="I9">
+        <v>206</v>
+      </c>
+      <c r="I9" t="s">
+        <v>242</v>
+      </c>
+      <c r="J9">
         <v>266</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>39</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
+        <v>65</v>
+      </c>
+      <c r="N9" t="s">
         <v>66</v>
       </c>
-      <c r="M9" t="s">
-        <v>67</v>
-      </c>
-      <c r="O9" t="s">
-        <v>40</v>
-      </c>
       <c r="P9" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>58</v>
+      </c>
+      <c r="R9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:19">
       <c r="A10">
         <v>1652</v>
       </c>
@@ -1443,34 +1522,34 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D10" t="s">
         <v>16</v>
       </c>
       <c r="E10" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="F10" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G10">
         <v>1</v>
       </c>
       <c r="H10" t="s">
-        <v>208</v>
-      </c>
-      <c r="I10">
+        <v>206</v>
+      </c>
+      <c r="J10">
         <v>236</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>69</v>
       </c>
-      <c r="O10" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17">
+      <c r="P10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19">
       <c r="A11">
         <v>1678</v>
       </c>
@@ -1478,16 +1557,16 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D11" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E11" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F11" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -1495,26 +1574,29 @@
       <c r="H11" t="s">
         <v>23</v>
       </c>
-      <c r="I11">
+      <c r="I11" t="s">
+        <v>238</v>
+      </c>
+      <c r="J11">
         <v>284</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <v>21</v>
       </c>
-      <c r="L11" t="s">
-        <v>161</v>
-      </c>
       <c r="M11" t="s">
-        <v>162</v>
-      </c>
-      <c r="O11" t="s">
+        <v>159</v>
+      </c>
+      <c r="N11" t="s">
+        <v>160</v>
+      </c>
+      <c r="P11" t="s">
         <v>24</v>
       </c>
-      <c r="P11" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17">
+      <c r="R11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19">
       <c r="A12">
         <v>1689</v>
       </c>
@@ -1522,46 +1604,49 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D12" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E12" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F12" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G12">
         <v>1</v>
       </c>
       <c r="H12" t="s">
-        <v>163</v>
-      </c>
-      <c r="I12">
+        <v>161</v>
+      </c>
+      <c r="I12" t="s">
+        <v>240</v>
+      </c>
+      <c r="J12">
         <v>263</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>299</v>
       </c>
-      <c r="K12">
+      <c r="L12">
         <v>36</v>
       </c>
-      <c r="M12" t="s">
-        <v>164</v>
-      </c>
       <c r="N12" t="s">
+        <v>162</v>
+      </c>
+      <c r="O12" t="s">
         <v>36</v>
       </c>
-      <c r="O12" t="s">
+      <c r="P12" t="s">
         <v>27</v>
       </c>
-      <c r="P12" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17">
+      <c r="R12" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19">
       <c r="A13">
         <v>1742</v>
       </c>
@@ -1569,40 +1654,43 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D13" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E13" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F13" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G13">
         <v>1</v>
       </c>
       <c r="H13" t="s">
-        <v>208</v>
-      </c>
-      <c r="I13">
+        <v>206</v>
+      </c>
+      <c r="I13" t="s">
+        <v>242</v>
+      </c>
+      <c r="J13">
         <v>266</v>
       </c>
-      <c r="K13">
+      <c r="L13">
         <v>39</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
+        <v>65</v>
+      </c>
+      <c r="N13" t="s">
         <v>66</v>
       </c>
-      <c r="M13" t="s">
-        <v>67</v>
-      </c>
-      <c r="O13" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17">
+      <c r="P13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19">
       <c r="A14">
         <v>1750</v>
       </c>
@@ -1610,40 +1698,43 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D14" t="s">
+        <v>163</v>
+      </c>
+      <c r="E14" t="s">
+        <v>219</v>
+      </c>
+      <c r="F14" t="s">
+        <v>142</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14" t="s">
+        <v>161</v>
+      </c>
+      <c r="I14" t="s">
+        <v>240</v>
+      </c>
+      <c r="J14">
+        <v>283</v>
+      </c>
+      <c r="L14">
+        <v>22</v>
+      </c>
+      <c r="M14" t="s">
+        <v>164</v>
+      </c>
+      <c r="N14" t="s">
         <v>165</v>
       </c>
-      <c r="E14" t="s">
-        <v>221</v>
-      </c>
-      <c r="F14" t="s">
-        <v>144</v>
-      </c>
-      <c r="G14">
-        <v>1</v>
-      </c>
-      <c r="H14" t="s">
-        <v>163</v>
-      </c>
-      <c r="I14">
-        <v>283</v>
-      </c>
-      <c r="K14">
-        <v>22</v>
-      </c>
-      <c r="L14" t="s">
-        <v>166</v>
-      </c>
-      <c r="M14" t="s">
-        <v>167</v>
-      </c>
-      <c r="O14" t="s">
+      <c r="P14" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:19">
       <c r="A15">
         <v>1785</v>
       </c>
@@ -1654,37 +1745,37 @@
         <v>33</v>
       </c>
       <c r="D15" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E15" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="F15" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G15">
         <v>1</v>
       </c>
       <c r="H15" t="s">
-        <v>208</v>
-      </c>
-      <c r="I15">
+        <v>206</v>
+      </c>
+      <c r="I15" t="s">
+        <v>241</v>
+      </c>
+      <c r="J15">
         <v>277</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <v>299</v>
       </c>
-      <c r="K15">
+      <c r="L15">
         <v>22</v>
       </c>
-      <c r="O15" t="s">
-        <v>59</v>
-      </c>
       <c r="P15" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19">
       <c r="A16">
         <v>1786</v>
       </c>
@@ -1692,31 +1783,34 @@
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E16" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F16" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G16">
         <v>1</v>
       </c>
       <c r="H16" t="s">
-        <v>175</v>
-      </c>
-      <c r="I16">
+        <v>173</v>
+      </c>
+      <c r="I16" t="s">
+        <v>243</v>
+      </c>
+      <c r="J16">
         <v>278</v>
       </c>
-      <c r="K16">
+      <c r="L16">
         <v>27</v>
       </c>
-      <c r="O16" t="s">
+      <c r="P16" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:17">
+    <row r="17" spans="1:19">
       <c r="A17">
         <v>1793</v>
       </c>
@@ -1724,37 +1818,40 @@
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E17" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="F17" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G17">
         <v>0</v>
       </c>
       <c r="H17" t="s">
-        <v>208</v>
-      </c>
-      <c r="I17">
+        <v>206</v>
+      </c>
+      <c r="I17" t="s">
+        <v>240</v>
+      </c>
+      <c r="J17">
         <v>286</v>
       </c>
-      <c r="K17">
+      <c r="L17">
         <v>19</v>
       </c>
-      <c r="L17" t="s">
+      <c r="M17" t="s">
+        <v>106</v>
+      </c>
+      <c r="N17" t="s">
         <v>37</v>
       </c>
-      <c r="M17" t="s">
-        <v>38</v>
-      </c>
-      <c r="O17" t="s">
+      <c r="P17" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:17">
+    <row r="18" spans="1:19">
       <c r="A18">
         <v>1799</v>
       </c>
@@ -1762,40 +1859,43 @@
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D18" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E18" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F18" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G18">
         <v>1</v>
       </c>
       <c r="H18" t="s">
-        <v>208</v>
-      </c>
-      <c r="I18">
+        <v>206</v>
+      </c>
+      <c r="I18" t="s">
         <v>242</v>
       </c>
       <c r="J18">
+        <v>242</v>
+      </c>
+      <c r="K18">
         <v>300</v>
       </c>
-      <c r="K18">
+      <c r="L18">
         <v>58</v>
       </c>
-      <c r="O18" t="s">
-        <v>40</v>
-      </c>
       <c r="P18" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17">
+        <v>39</v>
+      </c>
+      <c r="R18" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19">
       <c r="A19">
         <v>1829</v>
       </c>
@@ -1803,37 +1903,40 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D19" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E19" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="F19" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G19">
         <v>1</v>
       </c>
       <c r="H19" t="s">
-        <v>208</v>
-      </c>
-      <c r="I19">
+        <v>206</v>
+      </c>
+      <c r="I19" t="s">
+        <v>244</v>
+      </c>
+      <c r="J19">
         <v>268</v>
       </c>
-      <c r="K19">
+      <c r="L19">
         <v>37</v>
       </c>
-      <c r="O19" t="s">
-        <v>54</v>
-      </c>
       <c r="P19" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17">
+        <v>53</v>
+      </c>
+      <c r="R19" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19">
       <c r="A20">
         <v>1841</v>
       </c>
@@ -1841,40 +1944,43 @@
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D20" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E20" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F20" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G20">
         <v>1</v>
       </c>
       <c r="H20" t="s">
-        <v>208</v>
-      </c>
-      <c r="I20">
+        <v>206</v>
+      </c>
+      <c r="I20" t="s">
+        <v>242</v>
+      </c>
+      <c r="J20">
         <v>273</v>
       </c>
-      <c r="K20">
+      <c r="L20">
         <v>32</v>
       </c>
-      <c r="L20" t="s">
+      <c r="M20" t="s">
+        <v>65</v>
+      </c>
+      <c r="N20" t="s">
         <v>66</v>
       </c>
-      <c r="M20" t="s">
-        <v>67</v>
-      </c>
-      <c r="O20" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17">
+      <c r="P20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19">
       <c r="A21">
         <v>1782</v>
       </c>
@@ -1882,37 +1988,40 @@
         <v>0.97993311036789299</v>
       </c>
       <c r="C21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D21" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E21" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F21" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G21">
         <v>1</v>
       </c>
       <c r="H21" t="s">
-        <v>163</v>
-      </c>
-      <c r="I21">
+        <v>161</v>
+      </c>
+      <c r="I21" t="s">
+        <v>240</v>
+      </c>
+      <c r="J21">
         <v>260</v>
       </c>
-      <c r="K21">
+      <c r="L21">
         <v>45</v>
       </c>
-      <c r="O21" t="s">
-        <v>46</v>
-      </c>
       <c r="P21" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17">
+        <v>45</v>
+      </c>
+      <c r="R21" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19">
       <c r="A22">
         <v>274</v>
       </c>
@@ -1920,37 +2029,40 @@
         <v>0.96989966555183904</v>
       </c>
       <c r="C22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E22" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F22" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G22">
         <v>1</v>
       </c>
       <c r="H22" t="s">
-        <v>208</v>
-      </c>
-      <c r="I22">
+        <v>206</v>
+      </c>
+      <c r="I22" t="s">
+        <v>239</v>
+      </c>
+      <c r="J22">
         <v>283</v>
       </c>
-      <c r="K22">
+      <c r="L22">
         <v>22</v>
       </c>
-      <c r="L22" t="s">
-        <v>169</v>
-      </c>
       <c r="M22" t="s">
-        <v>78</v>
-      </c>
-      <c r="O22" t="s">
+        <v>167</v>
+      </c>
+      <c r="N22" t="s">
+        <v>77</v>
+      </c>
+      <c r="P22" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:17">
+    <row r="23" spans="1:19">
       <c r="A23">
         <v>1684</v>
       </c>
@@ -1958,40 +2070,43 @@
         <v>0.96989966555183904</v>
       </c>
       <c r="C23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D23" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E23" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F23" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G23">
         <v>1</v>
       </c>
       <c r="H23" t="s">
-        <v>208</v>
-      </c>
-      <c r="I23">
+        <v>206</v>
+      </c>
+      <c r="I23" t="s">
+        <v>241</v>
+      </c>
+      <c r="J23">
         <v>260</v>
       </c>
-      <c r="K23">
+      <c r="L23">
         <v>45</v>
       </c>
-      <c r="N23" t="s">
-        <v>171</v>
-      </c>
       <c r="O23" t="s">
-        <v>69</v>
+        <v>169</v>
       </c>
       <c r="P23" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17">
+        <v>68</v>
+      </c>
+      <c r="R23" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19">
       <c r="A24">
         <v>1831</v>
       </c>
@@ -1999,22 +2114,25 @@
         <v>0.89966555183946395</v>
       </c>
       <c r="C24" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D24" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E24" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F24" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:17">
+      <c r="I24" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19">
       <c r="A25">
         <v>2</v>
       </c>
@@ -2028,31 +2146,34 @@
         <v>13</v>
       </c>
       <c r="E25" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F25" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G25">
         <v>1</v>
       </c>
       <c r="H25" t="s">
-        <v>209</v>
-      </c>
-      <c r="I25">
+        <v>207</v>
+      </c>
+      <c r="I25" t="s">
+        <v>232</v>
+      </c>
+      <c r="J25">
         <v>208</v>
       </c>
-      <c r="K25">
+      <c r="L25">
         <v>97</v>
       </c>
-      <c r="O25" t="s">
+      <c r="P25" t="s">
         <v>14</v>
       </c>
-      <c r="P25" t="s">
+      <c r="R25" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:17">
+    <row r="26" spans="1:19">
       <c r="A26">
         <v>1752</v>
       </c>
@@ -2060,40 +2181,43 @@
         <v>0.86956521739130399</v>
       </c>
       <c r="C26" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D26" t="s">
         <v>16</v>
       </c>
       <c r="F26" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G26">
         <v>1</v>
       </c>
       <c r="H26" t="s">
-        <v>208</v>
-      </c>
-      <c r="I26">
+        <v>206</v>
+      </c>
+      <c r="I26" t="s">
+        <v>242</v>
+      </c>
+      <c r="J26">
         <v>244</v>
       </c>
-      <c r="J26">
+      <c r="K26">
         <v>300</v>
       </c>
-      <c r="K26">
+      <c r="L26">
         <v>56</v>
       </c>
-      <c r="N26" t="s">
-        <v>88</v>
-      </c>
       <c r="O26" t="s">
-        <v>40</v>
+        <v>87</v>
       </c>
       <c r="P26" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17">
+        <v>39</v>
+      </c>
+      <c r="R26" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19">
       <c r="A27">
         <v>1546</v>
       </c>
@@ -2101,43 +2225,46 @@
         <v>0.85618729096989898</v>
       </c>
       <c r="C27" t="s">
+        <v>89</v>
+      </c>
+      <c r="D27" t="s">
+        <v>170</v>
+      </c>
+      <c r="E27" t="s">
+        <v>195</v>
+      </c>
+      <c r="F27" t="s">
+        <v>142</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27" t="s">
+        <v>206</v>
+      </c>
+      <c r="I27" t="s">
+        <v>239</v>
+      </c>
+      <c r="J27">
+        <v>256</v>
+      </c>
+      <c r="L27">
+        <v>49</v>
+      </c>
+      <c r="M27" t="s">
+        <v>237</v>
+      </c>
+      <c r="O27" t="s">
+        <v>171</v>
+      </c>
+      <c r="P27" t="s">
+        <v>32</v>
+      </c>
+      <c r="R27" t="s">
         <v>90</v>
       </c>
-      <c r="D27" t="s">
-        <v>172</v>
-      </c>
-      <c r="E27" t="s">
-        <v>197</v>
-      </c>
-      <c r="F27" t="s">
-        <v>144</v>
-      </c>
-      <c r="G27">
-        <v>1</v>
-      </c>
-      <c r="H27" t="s">
-        <v>208</v>
-      </c>
-      <c r="I27">
-        <v>256</v>
-      </c>
-      <c r="K27">
-        <v>49</v>
-      </c>
-      <c r="L27" t="s">
-        <v>232</v>
-      </c>
-      <c r="N27" t="s">
-        <v>173</v>
-      </c>
-      <c r="O27" t="s">
-        <v>32</v>
-      </c>
-      <c r="P27" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17">
+    </row>
+    <row r="28" spans="1:19">
       <c r="A28">
         <v>1716</v>
       </c>
@@ -2145,37 +2272,40 @@
         <v>0.83612040133779197</v>
       </c>
       <c r="C28" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D28" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E28" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F28" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G28">
         <v>1</v>
       </c>
       <c r="H28" t="s">
-        <v>208</v>
-      </c>
-      <c r="I28">
+        <v>206</v>
+      </c>
+      <c r="I28" t="s">
+        <v>242</v>
+      </c>
+      <c r="J28">
         <v>265</v>
       </c>
-      <c r="J28">
+      <c r="K28">
         <v>300</v>
       </c>
-      <c r="K28">
+      <c r="L28">
         <v>35</v>
       </c>
-      <c r="O28" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17">
+      <c r="P28" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19">
       <c r="A29">
         <v>1745</v>
       </c>
@@ -2183,37 +2313,40 @@
         <v>0.83612040133779197</v>
       </c>
       <c r="C29" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F29" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G29">
         <v>1</v>
       </c>
       <c r="H29" t="s">
-        <v>208</v>
-      </c>
-      <c r="I29">
+        <v>206</v>
+      </c>
+      <c r="I29" t="s">
+        <v>244</v>
+      </c>
+      <c r="J29">
         <v>217</v>
       </c>
-      <c r="J29">
+      <c r="K29">
         <v>298</v>
       </c>
-      <c r="K29">
+      <c r="L29">
         <v>81</v>
       </c>
-      <c r="O29" t="s">
+      <c r="P29" t="s">
         <v>18</v>
       </c>
-      <c r="P29" t="s">
-        <v>121</v>
-      </c>
-      <c r="Q29" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17">
+      <c r="R29" t="s">
+        <v>236</v>
+      </c>
+      <c r="S29" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19">
       <c r="A30">
         <v>1919</v>
       </c>
@@ -2221,10 +2354,10 @@
         <v>0.79933110367892901</v>
       </c>
       <c r="C30" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F30" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G30">
         <v>1</v>
@@ -2232,26 +2365,29 @@
       <c r="H30" t="s">
         <v>23</v>
       </c>
-      <c r="I30">
+      <c r="I30" t="s">
+        <v>238</v>
+      </c>
+      <c r="J30">
         <v>259</v>
       </c>
-      <c r="J30">
+      <c r="K30">
         <v>283</v>
       </c>
-      <c r="K30">
+      <c r="L30">
         <v>24</v>
       </c>
-      <c r="O30" t="s">
+      <c r="P30" t="s">
         <v>24</v>
       </c>
-      <c r="P30" t="s">
-        <v>195</v>
-      </c>
-      <c r="Q30" t="s">
+      <c r="R30" t="s">
+        <v>193</v>
+      </c>
+      <c r="S30" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:17">
+    <row r="31" spans="1:19">
       <c r="A31">
         <v>1579</v>
       </c>
@@ -2259,37 +2395,40 @@
         <v>0.77257525083612</v>
       </c>
       <c r="C31" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D31" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E31" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F31" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G31">
         <v>1</v>
       </c>
       <c r="H31" t="s">
-        <v>210</v>
-      </c>
-      <c r="I31">
+        <v>208</v>
+      </c>
+      <c r="I31" t="s">
+        <v>246</v>
+      </c>
+      <c r="J31">
         <v>257</v>
       </c>
-      <c r="J31">
+      <c r="K31">
         <v>300</v>
       </c>
-      <c r="K31">
+      <c r="L31">
         <v>43</v>
       </c>
-      <c r="O31" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17">
+      <c r="P31" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19">
       <c r="A32">
         <v>1559</v>
       </c>
@@ -2297,28 +2436,31 @@
         <v>0.74581939799331098</v>
       </c>
       <c r="C32" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D32" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E32" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F32" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G32">
         <v>0</v>
       </c>
       <c r="H32" t="s">
-        <v>95</v>
-      </c>
-      <c r="O32" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17">
+        <v>94</v>
+      </c>
+      <c r="I32" t="s">
+        <v>245</v>
+      </c>
+      <c r="P32" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19">
       <c r="A33">
         <v>507</v>
       </c>
@@ -2326,34 +2468,37 @@
         <v>0.73913043478260798</v>
       </c>
       <c r="C33" t="s">
+        <v>61</v>
+      </c>
+      <c r="D33" t="s">
+        <v>155</v>
+      </c>
+      <c r="E33" t="s">
+        <v>172</v>
+      </c>
+      <c r="F33" t="s">
+        <v>142</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+      <c r="H33" t="s">
+        <v>173</v>
+      </c>
+      <c r="I33" t="s">
+        <v>243</v>
+      </c>
+      <c r="M33" t="s">
         <v>62</v>
       </c>
-      <c r="D33" t="s">
-        <v>157</v>
-      </c>
-      <c r="E33" t="s">
-        <v>174</v>
-      </c>
-      <c r="F33" t="s">
-        <v>144</v>
-      </c>
-      <c r="G33">
-        <v>1</v>
-      </c>
-      <c r="H33" t="s">
-        <v>175</v>
-      </c>
-      <c r="L33" t="s">
-        <v>63</v>
-      </c>
-      <c r="M33" t="s">
+      <c r="N33" t="s">
         <v>34</v>
       </c>
-      <c r="O33" t="s">
+      <c r="P33" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:17">
+    <row r="34" spans="1:19">
       <c r="A34">
         <v>1647</v>
       </c>
@@ -2361,37 +2506,40 @@
         <v>0.73913043478260798</v>
       </c>
       <c r="C34" t="s">
+        <v>99</v>
+      </c>
+      <c r="D34" t="s">
+        <v>201</v>
+      </c>
+      <c r="E34" t="s">
+        <v>195</v>
+      </c>
+      <c r="F34" t="s">
+        <v>142</v>
+      </c>
+      <c r="G34">
+        <v>1</v>
+      </c>
+      <c r="H34" t="s">
+        <v>173</v>
+      </c>
+      <c r="I34" t="s">
+        <v>243</v>
+      </c>
+      <c r="N34" t="s">
+        <v>34</v>
+      </c>
+      <c r="O34" t="s">
         <v>100</v>
       </c>
-      <c r="D34" t="s">
-        <v>203</v>
-      </c>
-      <c r="E34" t="s">
-        <v>197</v>
-      </c>
-      <c r="F34" t="s">
-        <v>144</v>
-      </c>
-      <c r="G34">
-        <v>1</v>
-      </c>
-      <c r="H34" t="s">
-        <v>175</v>
-      </c>
-      <c r="M34" t="s">
-        <v>34</v>
-      </c>
-      <c r="N34" t="s">
-        <v>101</v>
-      </c>
-      <c r="O34" t="s">
+      <c r="P34" t="s">
         <v>26</v>
       </c>
-      <c r="P34" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17">
+      <c r="R34" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19">
       <c r="A35">
         <v>1531</v>
       </c>
@@ -2399,37 +2547,40 @@
         <v>0.72240802675585203</v>
       </c>
       <c r="C35" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D35" t="s">
         <v>16</v>
       </c>
       <c r="E35" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F35" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G35">
         <v>1</v>
       </c>
       <c r="H35" t="s">
-        <v>175</v>
-      </c>
-      <c r="I35">
+        <v>173</v>
+      </c>
+      <c r="I35" t="s">
+        <v>240</v>
+      </c>
+      <c r="J35">
         <v>254</v>
       </c>
-      <c r="K35">
+      <c r="L35">
         <v>51</v>
       </c>
-      <c r="M35" t="s">
-        <v>134</v>
-      </c>
-      <c r="O35" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17">
+      <c r="N35" t="s">
+        <v>132</v>
+      </c>
+      <c r="P35" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19">
       <c r="A36">
         <v>1643</v>
       </c>
@@ -2437,37 +2588,40 @@
         <v>0.70903010033444802</v>
       </c>
       <c r="C36" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E36" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F36" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G36">
         <v>0</v>
       </c>
       <c r="H36" t="s">
-        <v>175</v>
-      </c>
-      <c r="I36">
+        <v>173</v>
+      </c>
+      <c r="I36" t="s">
+        <v>243</v>
+      </c>
+      <c r="J36">
         <v>275</v>
       </c>
-      <c r="K36">
+      <c r="L36">
         <v>30</v>
       </c>
-      <c r="L36" t="s">
-        <v>176</v>
-      </c>
       <c r="M36" t="s">
-        <v>100</v>
-      </c>
-      <c r="O36" t="s">
+        <v>174</v>
+      </c>
+      <c r="N36" t="s">
+        <v>99</v>
+      </c>
+      <c r="P36" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="37" spans="1:17">
+    <row r="37" spans="1:19">
       <c r="A37">
         <v>1764</v>
       </c>
@@ -2475,31 +2629,34 @@
         <v>0.70903010033444802</v>
       </c>
       <c r="C37" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D37" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E37" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F37" t="s">
+        <v>178</v>
+      </c>
+      <c r="G37">
+        <v>1</v>
+      </c>
+      <c r="H37" t="s">
+        <v>41</v>
+      </c>
+      <c r="I37" t="s">
+        <v>247</v>
+      </c>
+      <c r="P37" t="s">
+        <v>179</v>
+      </c>
+      <c r="R37" t="s">
         <v>180</v>
       </c>
-      <c r="G37">
-        <v>1</v>
-      </c>
-      <c r="H37" t="s">
-        <v>42</v>
-      </c>
-      <c r="O37" t="s">
-        <v>181</v>
-      </c>
-      <c r="P37" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17">
+    </row>
+    <row r="38" spans="1:19">
       <c r="A38">
         <v>1834</v>
       </c>
@@ -2507,37 +2664,40 @@
         <v>0.70568561872909696</v>
       </c>
       <c r="C38" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D38" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E38" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F38" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G38">
         <v>1</v>
       </c>
       <c r="H38" t="s">
-        <v>175</v>
-      </c>
-      <c r="I38">
+        <v>173</v>
+      </c>
+      <c r="I38" t="s">
+        <v>243</v>
+      </c>
+      <c r="J38">
         <v>268</v>
       </c>
-      <c r="K38">
+      <c r="L38">
         <v>37</v>
       </c>
-      <c r="M38" t="s">
+      <c r="N38" t="s">
         <v>34</v>
       </c>
-      <c r="O38" t="s">
+      <c r="P38" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="1:17">
+    <row r="39" spans="1:19">
       <c r="A39">
         <v>1854</v>
       </c>
@@ -2545,37 +2705,40 @@
         <v>0.69565217391304301</v>
       </c>
       <c r="C39" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D39" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E39" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="F39" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G39">
         <v>1</v>
       </c>
       <c r="H39" t="s">
-        <v>208</v>
-      </c>
-      <c r="I39">
+        <v>206</v>
+      </c>
+      <c r="I39" t="s">
+        <v>242</v>
+      </c>
+      <c r="J39">
         <v>270</v>
       </c>
-      <c r="J39">
+      <c r="K39">
         <v>300</v>
       </c>
-      <c r="K39">
+      <c r="L39">
         <v>30</v>
       </c>
-      <c r="O39" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17">
+      <c r="P39" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19">
       <c r="A40">
         <v>1928</v>
       </c>
@@ -2583,37 +2746,40 @@
         <v>0.66555183946488194</v>
       </c>
       <c r="C40" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D40" t="s">
         <v>16</v>
       </c>
       <c r="E40" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F40" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G40">
         <v>1</v>
       </c>
       <c r="H40" t="s">
-        <v>208</v>
-      </c>
-      <c r="I40">
+        <v>206</v>
+      </c>
+      <c r="I40" t="s">
+        <v>239</v>
+      </c>
+      <c r="J40">
         <v>282</v>
       </c>
-      <c r="K40">
+      <c r="L40">
         <v>23</v>
       </c>
-      <c r="M40" t="s">
-        <v>90</v>
-      </c>
-      <c r="O40" t="s">
+      <c r="N40" t="s">
+        <v>89</v>
+      </c>
+      <c r="P40" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="41" spans="1:17">
+    <row r="41" spans="1:19">
       <c r="A41">
         <v>1691</v>
       </c>
@@ -2621,34 +2787,37 @@
         <v>0.65551839464882899</v>
       </c>
       <c r="C41" t="s">
+        <v>107</v>
+      </c>
+      <c r="E41" t="s">
+        <v>195</v>
+      </c>
+      <c r="F41" t="s">
+        <v>142</v>
+      </c>
+      <c r="G41">
+        <v>1</v>
+      </c>
+      <c r="H41" t="s">
+        <v>207</v>
+      </c>
+      <c r="I41" t="s">
+        <v>232</v>
+      </c>
+      <c r="J41">
+        <v>267</v>
+      </c>
+      <c r="L41">
+        <v>38</v>
+      </c>
+      <c r="P41" t="s">
+        <v>59</v>
+      </c>
+      <c r="R41" t="s">
         <v>108</v>
       </c>
-      <c r="E41" t="s">
-        <v>197</v>
-      </c>
-      <c r="F41" t="s">
-        <v>144</v>
-      </c>
-      <c r="G41">
-        <v>1</v>
-      </c>
-      <c r="H41" t="s">
-        <v>209</v>
-      </c>
-      <c r="I41">
-        <v>267</v>
-      </c>
-      <c r="K41">
-        <v>38</v>
-      </c>
-      <c r="O41" t="s">
-        <v>60</v>
-      </c>
-      <c r="P41" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="42" spans="1:17">
+    </row>
+    <row r="42" spans="1:19">
       <c r="A42">
         <v>1602</v>
       </c>
@@ -2656,37 +2825,37 @@
         <v>0.63879598662207304</v>
       </c>
       <c r="C42" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D42" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E42" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F42" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G42">
         <v>1</v>
       </c>
       <c r="H42" t="s">
-        <v>208</v>
-      </c>
-      <c r="I42">
+        <v>206</v>
+      </c>
+      <c r="J42">
         <v>216</v>
       </c>
-      <c r="J42">
+      <c r="K42">
         <v>300</v>
       </c>
-      <c r="K42">
+      <c r="L42">
         <v>84</v>
       </c>
-      <c r="O42" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="43" spans="1:17">
+      <c r="P42" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19">
       <c r="A43">
         <v>1830</v>
       </c>
@@ -2694,10 +2863,10 @@
         <v>0.62207357859531698</v>
       </c>
       <c r="C43" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F43" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G43">
         <v>1</v>
@@ -2705,29 +2874,32 @@
       <c r="H43" t="s">
         <v>23</v>
       </c>
-      <c r="I43">
+      <c r="I43" t="s">
+        <v>238</v>
+      </c>
+      <c r="J43">
         <v>276</v>
       </c>
-      <c r="J43">
+      <c r="K43">
         <v>298</v>
       </c>
-      <c r="K43">
+      <c r="L43">
         <v>22</v>
       </c>
-      <c r="L43" t="s">
-        <v>161</v>
-      </c>
       <c r="M43" t="s">
-        <v>162</v>
-      </c>
-      <c r="O43" t="s">
+        <v>159</v>
+      </c>
+      <c r="N43" t="s">
+        <v>160</v>
+      </c>
+      <c r="P43" t="s">
         <v>24</v>
       </c>
-      <c r="Q43" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="44" spans="1:17">
+      <c r="S43" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19">
       <c r="A44">
         <v>1608</v>
       </c>
@@ -2735,31 +2907,34 @@
         <v>0.61872909698996603</v>
       </c>
       <c r="C44" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D44" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E44" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F44" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G44">
         <v>1</v>
       </c>
       <c r="H44" t="s">
-        <v>208</v>
-      </c>
-      <c r="O44" t="s">
-        <v>51</v>
+        <v>206</v>
+      </c>
+      <c r="I44" t="s">
+        <v>239</v>
       </c>
       <c r="P44" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="45" spans="1:17">
+        <v>50</v>
+      </c>
+      <c r="R44" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19">
       <c r="A45">
         <v>1868</v>
       </c>
@@ -2767,37 +2942,40 @@
         <v>0.61872909698996603</v>
       </c>
       <c r="C45" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D45" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E45" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F45" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G45">
         <v>1</v>
       </c>
       <c r="H45" t="s">
-        <v>163</v>
-      </c>
-      <c r="I45">
+        <v>161</v>
+      </c>
+      <c r="I45" t="s">
+        <v>240</v>
+      </c>
+      <c r="J45">
         <v>230</v>
       </c>
-      <c r="J45">
+      <c r="K45">
         <v>299</v>
       </c>
-      <c r="K45">
+      <c r="L45">
         <v>69</v>
       </c>
-      <c r="O45" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="46" spans="1:17">
+      <c r="P45" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19">
       <c r="A46">
         <v>1666</v>
       </c>
@@ -2805,13 +2983,13 @@
         <v>0.60535117056856103</v>
       </c>
       <c r="C46" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E46" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F46" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G46">
         <v>1</v>
@@ -2819,20 +2997,23 @@
       <c r="H46" t="s">
         <v>23</v>
       </c>
-      <c r="I46">
+      <c r="I46" t="s">
+        <v>232</v>
+      </c>
+      <c r="J46">
         <v>175</v>
       </c>
-      <c r="J46">
+      <c r="K46">
         <v>252</v>
       </c>
-      <c r="K46">
+      <c r="L46">
         <v>77</v>
       </c>
-      <c r="O46" t="s">
+      <c r="P46" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="47" spans="1:17">
+    <row r="47" spans="1:19">
       <c r="A47">
         <v>1899</v>
       </c>
@@ -2840,37 +3021,40 @@
         <v>0.57190635451505001</v>
       </c>
       <c r="C47" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D47" t="s">
         <v>35</v>
       </c>
       <c r="E47" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="F47" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G47">
         <v>0</v>
       </c>
       <c r="H47" t="s">
-        <v>210</v>
-      </c>
-      <c r="I47">
+        <v>208</v>
+      </c>
+      <c r="I47" t="s">
+        <v>246</v>
+      </c>
+      <c r="J47">
         <v>276</v>
       </c>
-      <c r="K47">
+      <c r="L47">
         <v>29</v>
       </c>
-      <c r="M47" t="s">
-        <v>83</v>
-      </c>
-      <c r="O47" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="48" spans="1:17">
+      <c r="N47" t="s">
+        <v>82</v>
+      </c>
+      <c r="P47" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19">
       <c r="A48">
         <v>1523</v>
       </c>
@@ -2878,37 +3062,40 @@
         <v>0.56187290969899595</v>
       </c>
       <c r="C48" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D48" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E48" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F48" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G48">
         <v>1</v>
       </c>
       <c r="H48" t="s">
-        <v>208</v>
-      </c>
-      <c r="I48">
+        <v>206</v>
+      </c>
+      <c r="I48" t="s">
+        <v>238</v>
+      </c>
+      <c r="J48">
         <v>278</v>
       </c>
-      <c r="J48">
+      <c r="K48">
         <v>300</v>
       </c>
-      <c r="K48">
+      <c r="L48">
         <v>22</v>
       </c>
-      <c r="O48" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="49" spans="1:17">
+      <c r="P48" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19">
       <c r="A49">
         <v>1574</v>
       </c>
@@ -2922,28 +3109,31 @@
         <v>35</v>
       </c>
       <c r="E49" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="F49" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G49">
         <v>0</v>
       </c>
       <c r="H49" t="s">
-        <v>208</v>
-      </c>
-      <c r="I49">
+        <v>206</v>
+      </c>
+      <c r="I49" t="s">
+        <v>238</v>
+      </c>
+      <c r="J49">
         <v>290</v>
       </c>
-      <c r="K49">
+      <c r="L49">
         <v>15</v>
       </c>
-      <c r="O49" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="50" spans="1:17">
+      <c r="P49" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19">
       <c r="A50">
         <v>1920</v>
       </c>
@@ -2951,7 +3141,7 @@
         <v>0.558528428093645</v>
       </c>
       <c r="C50" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F50" t="s">
         <v>28</v>
@@ -2962,29 +3152,32 @@
       <c r="H50" t="s">
         <v>28</v>
       </c>
-      <c r="I50">
+      <c r="I50" t="s">
+        <v>245</v>
+      </c>
+      <c r="J50">
         <v>267</v>
       </c>
-      <c r="J50" s="1">
+      <c r="K50" s="1">
         <v>298</v>
       </c>
-      <c r="K50">
+      <c r="L50">
         <v>32</v>
       </c>
-      <c r="M50" t="s">
-        <v>185</v>
-      </c>
-      <c r="O50" t="s">
+      <c r="N50" t="s">
+        <v>183</v>
+      </c>
+      <c r="P50" t="s">
         <v>28</v>
       </c>
-      <c r="P50" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q50" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="51" spans="1:17">
+      <c r="R50" t="s">
+        <v>75</v>
+      </c>
+      <c r="S50" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19">
       <c r="A51">
         <v>1605</v>
       </c>
@@ -2992,40 +3185,43 @@
         <v>0.551839464882943</v>
       </c>
       <c r="C51" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D51" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E51" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F51" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G51">
         <v>1</v>
       </c>
       <c r="H51" t="s">
-        <v>210</v>
-      </c>
-      <c r="I51">
+        <v>208</v>
+      </c>
+      <c r="I51" t="s">
+        <v>246</v>
+      </c>
+      <c r="J51">
         <v>281</v>
       </c>
-      <c r="J51">
+      <c r="K51">
         <v>300</v>
       </c>
-      <c r="K51">
+      <c r="L51">
         <v>19</v>
       </c>
-      <c r="M51" t="s">
-        <v>83</v>
-      </c>
-      <c r="O51" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="52" spans="1:17">
+      <c r="N51" t="s">
+        <v>82</v>
+      </c>
+      <c r="P51" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19">
       <c r="A52">
         <v>1877</v>
       </c>
@@ -3033,37 +3229,40 @@
         <v>0.551839464882943</v>
       </c>
       <c r="C52" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E52" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F52" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G52">
         <v>1</v>
       </c>
       <c r="H52" t="s">
-        <v>163</v>
-      </c>
-      <c r="I52">
+        <v>161</v>
+      </c>
+      <c r="I52" t="s">
+        <v>240</v>
+      </c>
+      <c r="J52">
         <v>295</v>
       </c>
-      <c r="K52">
+      <c r="L52">
         <v>10</v>
       </c>
-      <c r="L52" t="s">
+      <c r="M52" t="s">
+        <v>106</v>
+      </c>
+      <c r="N52" t="s">
         <v>37</v>
       </c>
-      <c r="M52" t="s">
-        <v>38</v>
-      </c>
-      <c r="O52" t="s">
+      <c r="P52" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="53" spans="1:17">
+    <row r="53" spans="1:19">
       <c r="A53">
         <v>1874</v>
       </c>
@@ -3071,25 +3270,25 @@
         <v>0.53511705685618705</v>
       </c>
       <c r="C53" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E53" t="s">
+        <v>204</v>
+      </c>
+      <c r="F53" t="s">
+        <v>142</v>
+      </c>
+      <c r="G53">
+        <v>1</v>
+      </c>
+      <c r="H53" t="s">
         <v>206</v>
       </c>
-      <c r="F53" t="s">
-        <v>144</v>
-      </c>
-      <c r="G53">
-        <v>1</v>
-      </c>
-      <c r="H53" t="s">
-        <v>208</v>
-      </c>
-      <c r="O53" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="54" spans="1:17">
+      <c r="P53" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19">
       <c r="A54">
         <v>1497</v>
       </c>
@@ -3097,40 +3296,43 @@
         <v>0.49832775919732403</v>
       </c>
       <c r="C54" t="s">
+        <v>82</v>
+      </c>
+      <c r="D54" t="s">
+        <v>74</v>
+      </c>
+      <c r="E54" t="s">
+        <v>157</v>
+      </c>
+      <c r="F54" t="s">
+        <v>142</v>
+      </c>
+      <c r="G54">
+        <v>1</v>
+      </c>
+      <c r="H54" t="s">
+        <v>208</v>
+      </c>
+      <c r="I54" t="s">
+        <v>246</v>
+      </c>
+      <c r="J54">
+        <v>247</v>
+      </c>
+      <c r="L54">
+        <v>58</v>
+      </c>
+      <c r="O54" t="s">
+        <v>135</v>
+      </c>
+      <c r="P54" t="s">
+        <v>51</v>
+      </c>
+      <c r="R54" t="s">
         <v>83</v>
       </c>
-      <c r="D54" t="s">
-        <v>75</v>
-      </c>
-      <c r="E54" t="s">
-        <v>159</v>
-      </c>
-      <c r="F54" t="s">
-        <v>144</v>
-      </c>
-      <c r="G54">
-        <v>1</v>
-      </c>
-      <c r="H54" t="s">
-        <v>210</v>
-      </c>
-      <c r="I54">
-        <v>247</v>
-      </c>
-      <c r="K54">
-        <v>58</v>
-      </c>
-      <c r="N54" t="s">
-        <v>137</v>
-      </c>
-      <c r="O54" t="s">
-        <v>52</v>
-      </c>
-      <c r="P54" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="55" spans="1:17">
+    </row>
+    <row r="55" spans="1:19">
       <c r="A55">
         <v>1537</v>
       </c>
@@ -3138,31 +3340,34 @@
         <v>0.47826086956521702</v>
       </c>
       <c r="C55" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E55" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F55" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G55">
         <v>1</v>
       </c>
       <c r="H55" t="s">
-        <v>208</v>
-      </c>
-      <c r="I55">
+        <v>206</v>
+      </c>
+      <c r="I55" t="s">
+        <v>242</v>
+      </c>
+      <c r="J55">
         <v>282</v>
       </c>
-      <c r="K55">
+      <c r="L55">
         <v>23</v>
       </c>
-      <c r="O55" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="56" spans="1:17">
+      <c r="P55" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19">
       <c r="A56">
         <v>1476</v>
       </c>
@@ -3170,28 +3375,28 @@
         <v>0.47157190635451501</v>
       </c>
       <c r="C56" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E56" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F56" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G56">
         <v>1</v>
       </c>
       <c r="H56" t="s">
-        <v>208</v>
-      </c>
-      <c r="I56">
+        <v>206</v>
+      </c>
+      <c r="J56">
         <v>264</v>
       </c>
-      <c r="K56">
+      <c r="L56">
         <v>41</v>
       </c>
     </row>
-    <row r="57" spans="1:17">
+    <row r="57" spans="1:19">
       <c r="A57">
         <v>1607</v>
       </c>
@@ -3199,34 +3404,37 @@
         <v>0.46153846153846101</v>
       </c>
       <c r="C57" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D57" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F57" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G57">
         <v>1</v>
       </c>
       <c r="H57" t="s">
-        <v>163</v>
-      </c>
-      <c r="I57">
+        <v>161</v>
+      </c>
+      <c r="I57" t="s">
+        <v>240</v>
+      </c>
+      <c r="J57">
         <v>282</v>
       </c>
-      <c r="K57">
+      <c r="L57">
         <v>23</v>
       </c>
-      <c r="M57" t="s">
-        <v>55</v>
-      </c>
-      <c r="O57" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="58" spans="1:17">
+      <c r="N57" t="s">
+        <v>54</v>
+      </c>
+      <c r="P57" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19">
       <c r="A58">
         <v>1722</v>
       </c>
@@ -3234,10 +3442,10 @@
         <v>0.444816053511705</v>
       </c>
       <c r="C58" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F58" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G58">
         <v>1</v>
@@ -3245,8 +3453,11 @@
       <c r="H58" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="59" spans="1:17">
+      <c r="I58" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="59" spans="1:19">
       <c r="A59">
         <v>1692</v>
       </c>
@@ -3254,37 +3465,43 @@
         <v>0.441471571906354</v>
       </c>
       <c r="C59" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F59" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G59">
         <v>0</v>
       </c>
       <c r="H59" t="s">
-        <v>210</v>
-      </c>
-      <c r="I59">
+        <v>208</v>
+      </c>
+      <c r="I59" t="s">
+        <v>246</v>
+      </c>
+      <c r="J59">
         <v>256</v>
       </c>
-      <c r="J59">
+      <c r="K59">
         <v>283</v>
       </c>
-      <c r="K59">
+      <c r="L59">
         <v>27</v>
       </c>
-      <c r="O59" t="s">
+      <c r="P59" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q59" t="s">
         <v>24</v>
       </c>
-      <c r="P59" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q59" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="60" spans="1:17">
+      <c r="R59" t="s">
+        <v>57</v>
+      </c>
+      <c r="S59" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="60" spans="1:19">
       <c r="A60">
         <v>1926</v>
       </c>
@@ -3292,28 +3509,31 @@
         <v>0.438127090301003</v>
       </c>
       <c r="C60" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F60" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G60">
         <v>1</v>
       </c>
       <c r="H60" t="s">
-        <v>208</v>
-      </c>
-      <c r="I60">
+        <v>206</v>
+      </c>
+      <c r="I60" t="s">
+        <v>238</v>
+      </c>
+      <c r="J60">
         <v>284</v>
       </c>
-      <c r="K60">
+      <c r="L60">
         <v>21</v>
       </c>
-      <c r="M60" t="s">
+      <c r="N60" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="61" spans="1:17">
+    <row r="61" spans="1:19">
       <c r="A61">
         <v>1659</v>
       </c>
@@ -3321,37 +3541,40 @@
         <v>0.434782608695652</v>
       </c>
       <c r="C61" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D61" t="s">
+        <v>185</v>
+      </c>
+      <c r="E61" t="s">
+        <v>221</v>
+      </c>
+      <c r="F61" t="s">
+        <v>142</v>
+      </c>
+      <c r="G61">
+        <v>1</v>
+      </c>
+      <c r="H61" t="s">
+        <v>186</v>
+      </c>
+      <c r="I61" t="s">
+        <v>241</v>
+      </c>
+      <c r="J61">
+        <v>276</v>
+      </c>
+      <c r="K61">
+        <v>299</v>
+      </c>
+      <c r="L61">
+        <v>23</v>
+      </c>
+      <c r="P61" t="s">
         <v>187</v>
       </c>
-      <c r="E61" t="s">
-        <v>223</v>
-      </c>
-      <c r="F61" t="s">
-        <v>144</v>
-      </c>
-      <c r="G61">
-        <v>1</v>
-      </c>
-      <c r="H61" t="s">
-        <v>188</v>
-      </c>
-      <c r="I61">
-        <v>276</v>
-      </c>
-      <c r="J61">
-        <v>299</v>
-      </c>
-      <c r="K61">
-        <v>23</v>
-      </c>
-      <c r="O61" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="62" spans="1:17">
+    </row>
+    <row r="62" spans="1:19">
       <c r="A62">
         <v>637</v>
       </c>
@@ -3359,31 +3582,34 @@
         <v>0.42474916387959799</v>
       </c>
       <c r="C62" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F62" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G62">
         <v>0</v>
       </c>
       <c r="H62" t="s">
-        <v>208</v>
-      </c>
-      <c r="I62">
+        <v>206</v>
+      </c>
+      <c r="I62" t="s">
+        <v>242</v>
+      </c>
+      <c r="J62">
         <v>283</v>
       </c>
-      <c r="K62">
+      <c r="L62">
         <v>22</v>
       </c>
-      <c r="O62" t="s">
-        <v>41</v>
-      </c>
       <c r="P62" t="s">
+        <v>40</v>
+      </c>
+      <c r="R62" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="63" spans="1:17">
+    <row r="63" spans="1:19">
       <c r="A63">
         <v>1657</v>
       </c>
@@ -3391,37 +3617,40 @@
         <v>0.40133779264213998</v>
       </c>
       <c r="C63" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D63" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E63" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F63" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G63">
         <v>1</v>
       </c>
       <c r="H63" t="s">
-        <v>163</v>
-      </c>
-      <c r="I63">
+        <v>161</v>
+      </c>
+      <c r="I63" t="s">
+        <v>240</v>
+      </c>
+      <c r="J63">
         <v>267</v>
       </c>
-      <c r="K63">
+      <c r="L63">
         <v>38</v>
       </c>
-      <c r="M63" t="s">
-        <v>164</v>
-      </c>
-      <c r="O63" t="s">
+      <c r="N63" t="s">
+        <v>162</v>
+      </c>
+      <c r="P63" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="64" spans="1:17">
+    <row r="64" spans="1:19">
       <c r="A64">
         <v>1821</v>
       </c>
@@ -3429,34 +3658,37 @@
         <v>0.39799331103678898</v>
       </c>
       <c r="C64" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D64" t="s">
         <v>16</v>
       </c>
       <c r="E64" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F64" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G64">
         <v>1</v>
       </c>
       <c r="H64" t="s">
-        <v>211</v>
-      </c>
-      <c r="J64">
+        <v>209</v>
+      </c>
+      <c r="I64" t="s">
+        <v>240</v>
+      </c>
+      <c r="K64">
         <v>299</v>
       </c>
-      <c r="N64" t="s">
-        <v>190</v>
-      </c>
       <c r="O64" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="65" spans="1:16">
+        <v>188</v>
+      </c>
+      <c r="P64" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="65" spans="1:19">
       <c r="A65">
         <v>1852</v>
       </c>
@@ -3464,31 +3696,37 @@
         <v>0.39799331103678898</v>
       </c>
       <c r="C65" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D65" t="s">
         <v>17</v>
       </c>
       <c r="E65" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F65" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G65">
         <v>0</v>
       </c>
       <c r="H65" t="s">
-        <v>208</v>
-      </c>
-      <c r="O65" t="s">
-        <v>68</v>
+        <v>206</v>
+      </c>
+      <c r="I65" t="s">
+        <v>241</v>
       </c>
       <c r="P65" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="66" spans="1:16">
+        <v>67</v>
+      </c>
+      <c r="Q65" t="s">
+        <v>58</v>
+      </c>
+      <c r="R65" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="66" spans="1:19">
       <c r="A66">
         <v>1737</v>
       </c>
@@ -3496,31 +3734,34 @@
         <v>0.39464882943143798</v>
       </c>
       <c r="C66" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D66" t="s">
+        <v>112</v>
+      </c>
+      <c r="E66" t="s">
+        <v>189</v>
+      </c>
+      <c r="F66" t="s">
+        <v>142</v>
+      </c>
+      <c r="G66">
+        <v>1</v>
+      </c>
+      <c r="H66" t="s">
+        <v>78</v>
+      </c>
+      <c r="I66" t="s">
+        <v>245</v>
+      </c>
+      <c r="P66" t="s">
+        <v>24</v>
+      </c>
+      <c r="R66" t="s">
         <v>113</v>
       </c>
-      <c r="E66" t="s">
-        <v>191</v>
-      </c>
-      <c r="F66" t="s">
-        <v>144</v>
-      </c>
-      <c r="G66">
-        <v>1</v>
-      </c>
-      <c r="H66" t="s">
-        <v>79</v>
-      </c>
-      <c r="O66" t="s">
-        <v>24</v>
-      </c>
-      <c r="P66" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="67" spans="1:16">
+    </row>
+    <row r="67" spans="1:19">
       <c r="A67">
         <v>1744</v>
       </c>
@@ -3528,25 +3769,28 @@
         <v>0.38461538461538403</v>
       </c>
       <c r="C67" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F67" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G67">
         <v>0</v>
       </c>
       <c r="H67" t="s">
-        <v>163</v>
-      </c>
-      <c r="M67" t="s">
-        <v>230</v>
-      </c>
-      <c r="O67" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="68" spans="1:16">
+        <v>161</v>
+      </c>
+      <c r="I67" t="s">
+        <v>240</v>
+      </c>
+      <c r="N67" t="s">
+        <v>228</v>
+      </c>
+      <c r="P67" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="68" spans="1:19">
       <c r="A68">
         <v>1577</v>
       </c>
@@ -3554,28 +3798,31 @@
         <v>0.37792642140468202</v>
       </c>
       <c r="C68" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F68" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G68">
         <v>0</v>
       </c>
       <c r="H68" t="s">
-        <v>210</v>
-      </c>
-      <c r="I68">
+        <v>208</v>
+      </c>
+      <c r="I68" t="s">
+        <v>246</v>
+      </c>
+      <c r="J68">
         <v>274</v>
       </c>
-      <c r="K68">
+      <c r="L68">
         <v>31</v>
       </c>
-      <c r="O68" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="69" spans="1:16">
+      <c r="P68" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="69" spans="1:19">
       <c r="A69">
         <v>1541</v>
       </c>
@@ -3583,34 +3830,90 @@
         <v>0.35451505016722401</v>
       </c>
       <c r="C69" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F69" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G69">
         <v>1</v>
       </c>
       <c r="H69" t="s">
-        <v>163</v>
-      </c>
-      <c r="I69">
+        <v>161</v>
+      </c>
+      <c r="I69" t="s">
+        <v>240</v>
+      </c>
+      <c r="J69">
         <v>266</v>
       </c>
-      <c r="J69">
+      <c r="K69">
         <v>283</v>
       </c>
-      <c r="K69">
+      <c r="L69">
         <v>17</v>
       </c>
-      <c r="M69" t="s">
-        <v>164</v>
-      </c>
-      <c r="O69" t="s">
+      <c r="N69" t="s">
+        <v>162</v>
+      </c>
+      <c r="P69" t="s">
         <v>27</v>
       </c>
-      <c r="P69" t="s">
+      <c r="Q69" t="s">
+        <v>235</v>
+      </c>
+      <c r="R69" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="70" spans="1:19">
+      <c r="A70">
+        <v>411</v>
+      </c>
+      <c r="B70">
+        <v>0</v>
+      </c>
+      <c r="C70" t="s">
+        <v>106</v>
+      </c>
+      <c r="E70" t="s">
         <v>194</v>
+      </c>
+      <c r="F70" t="s">
+        <v>142</v>
+      </c>
+      <c r="G70">
+        <v>0</v>
+      </c>
+      <c r="H70" t="s">
+        <v>207</v>
+      </c>
+      <c r="I70" t="s">
+        <v>232</v>
+      </c>
+      <c r="J70">
+        <v>264</v>
+      </c>
+      <c r="K70">
+        <v>299</v>
+      </c>
+      <c r="L70">
+        <v>35</v>
+      </c>
+      <c r="N70" t="s">
+        <v>233</v>
+      </c>
+      <c r="P70" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q70" t="s">
+        <v>27</v>
+      </c>
+      <c r="R70" t="s">
+        <v>37</v>
+      </c>
+      <c r="S70" t="s">
+        <v>234</v>
       </c>
     </row>
   </sheetData>

</xml_diff>